<commit_message>
Second Script | SOP
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -41,109 +41,37 @@
     <t>other_phone</t>
   </si>
   <si>
-    <t>Solo Performances and Teacher Duets (Style 1)</t>
-  </si>
-  <si>
-    <t>Please choose the number of performers:</t>
-  </si>
-  <si>
-    <t>1. Performer Information</t>
-  </si>
-  <si>
-    <t>1. Performer Information First name</t>
-  </si>
-  <si>
-    <t>1. Performer Information Last name</t>
-  </si>
-  <si>
-    <t>1. Song 1</t>
-  </si>
-  <si>
-    <t>1. Song1 Length</t>
-  </si>
-  <si>
-    <t>1. Song1 Composer/Arranger</t>
-  </si>
-  <si>
-    <t>1. Song2</t>
-  </si>
-  <si>
-    <t>1. Song2 Length</t>
-  </si>
-  <si>
-    <t>1. Song2 Composer/Arranger</t>
-  </si>
-  <si>
-    <t>2. Performer Information</t>
-  </si>
-  <si>
-    <t>2. Performer Information First name</t>
-  </si>
-  <si>
-    <t>2. Performer Information Last name</t>
-  </si>
-  <si>
-    <t>2. Song 1</t>
-  </si>
-  <si>
-    <t>2. Song 1 Length</t>
-  </si>
-  <si>
-    <t>2. Song1 Composer/Arranger</t>
-  </si>
-  <si>
-    <t>2. Song 2</t>
-  </si>
-  <si>
-    <t>2. Song2 Length</t>
-  </si>
-  <si>
-    <t>2. Song2 Composer/Arranger</t>
-  </si>
-  <si>
-    <t>Justin (Test) Powley (Test)</t>
-  </si>
-  <si>
-    <t>Justin (Test)</t>
-  </si>
-  <si>
-    <t>Powley (Test)</t>
-  </si>
-  <si>
-    <t>jpowley@ualberta.ca</t>
+    <t>Solo Performances and Teacher Duets</t>
+  </si>
+  <si>
+    <t>Bands / Multi-Student Duets (2 Song Max):</t>
+  </si>
+  <si>
+    <t>Justin Powley</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>Powley</t>
+  </si>
+  <si>
+    <t>powleyjustin@gmail.com</t>
   </si>
   <si>
     <t>587-590-4107</t>
   </si>
   <si>
-    <t>1: First Name: Joseph, Last Name: Wardy, Song1 Title: Man In The Mirror, Song1 Length (minutes): 2, Song1 Composer/Arr.: Michael Jackson, Song2 Title: Can't Live Can't Die, Song2 Length (minutes): 3, Song2 Composer/Arr.: Edgy Artist #5, Song3 Title: Blips and Bloops, Song3 Length (minutes): 1:30, Song3 Composer/Arr.: Comma, Separated, Values, 2: First Name: Noseph, Last Name: Swardy, Song1 Title: Can in the career, Song1 Length (minutes): 3, Song1 Composer/Arr.: Not Jackson / Not Justin, Song2 Title: Less songs here, Song2 Length (minutes): 0.5, Song2 Composer/Arr.: Not a composer, 3: First Name: Finn, Last Name: Flynn, Song1 Title: Can't stop you now, Song1 Length (minutes): 1.2, Song1 Composer/Arr.: King</t>
-  </si>
-  <si>
-    <t>Justin Powley</t>
-  </si>
-  <si>
-    <t>Justin</t>
-  </si>
-  <si>
-    <t>Powley</t>
-  </si>
-  <si>
-    <t>Golden Slumbers</t>
-  </si>
-  <si>
-    <t>The Beatles</t>
-  </si>
-  <si>
-    <t>Memory Lane</t>
-  </si>
-  <si>
-    <t>Memory</t>
-  </si>
-  <si>
-    <t>Lane</t>
-  </si>
-  <si>
-    <t>Penny Lane</t>
+    <t>1: Performers (Full Names, Comma Separated): Justin Powley, Keith Cole, Fred Dreary, Pam Carlson, 2: Performers (Full Names, Comma Separated): Michael Jackson, Jermaine Jackson, Tito Jackson, Randy Jackson, Marlon Jackson</t>
+  </si>
+  <si>
+    <t>Performers (Full Names, Comma Separated): Ryan, Ashley, Connor</t>
+  </si>
+  <si>
+    <t>Band Name: The Cure, Performers (Full Names, Comma Separated): Robert Smith, Simon Gallup, Gary X, Roger O'Donnell, Positive Comment / Award: Best Band, Song1 Title: Pictures of You, Song1 Length (minutes): 8.5, Song1 Composer/Arr.: The Cure, Song1 Staging/Instruments: Vocals, Guitar, Bass, Piano, Song2 Title: Friday I'm in Love, Song2 Length (minutes): 3, Song2 Composer/Arr.: The Cure, Song2 Staging/Instruments: Vocals, Guitar, Bass, Piano, Second Keyboard</t>
+  </si>
+  <si>
+    <t>First Name: Single, Last Name: Entry, Positive Comment / Award: Yes, Song1 Title: Eleanor Rigby, Song1 Length (minutes): 2, Song1 Composer/Arr.: The Beatles, Song1 Staging/Instruments: Piano Solo</t>
   </si>
 </sst>
 </file>
@@ -497,15 +425,15 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:AB1"/>
+      <selection activeCell="A1" sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -536,131 +464,114 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>17158195</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45477.441400463</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="I2"/>
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>17158191</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45477.44125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>17150644</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45476.710821759</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>17150639</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45476.710393519</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2">
-        <v>16941419</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45463.505706019</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O2">
-        <v>3</v>
-      </c>
-      <c r="P2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X2">
-        <v>5</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z2"/>
-      <c r="AA2"/>
-      <c r="AB2"/>
+      <c r="J5"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>